<commit_message>
updated versions of mae and tc databases
</commit_message>
<xml_diff>
--- a/uc_mae.xlsx
+++ b/uc_mae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mario\trabajos2\innovación_docente_2024\ankipy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153582F-A7EB-48EF-B54B-4896790C36C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7825678C-19FA-417C-BB63-6DC290935C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LEEME" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="DatosExternos_4" localSheetId="4" hidden="1">ca!$A$1:$J$9</definedName>
     <definedName name="DatosExternos_4" localSheetId="5" hidden="1">cc!$A$1:$J$9</definedName>
-    <definedName name="DatosExternos_4" localSheetId="3" hidden="1">convertidores!$A$1:$J$9</definedName>
+    <definedName name="DatosExternos_4" localSheetId="3" hidden="1">convertidores!$A$1:$J$16</definedName>
     <definedName name="DatosExternos_4" localSheetId="1" hidden="1">intro!$A$1:$J$9</definedName>
     <definedName name="DatosExternos_4" localSheetId="2" hidden="1">mecanica!$A$1:$J$9</definedName>
     <definedName name="DatosExternos_4" localSheetId="6" hidden="1">reluctancia!$A$1:$J$9</definedName>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="120">
   <si>
     <t>slide</t>
   </si>
@@ -220,6 +220,237 @@
   </si>
   <si>
     <t>G875</t>
+  </si>
+  <si>
+    <t>What role is each block playing in the following diagram?</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>#intro</t>
+  </si>
+  <si>
+    <t>intro.1</t>
+  </si>
+  <si>
+    <t>pc.1</t>
+  </si>
+  <si>
+    <t>Considering you are in Spain, what is the peak value of the 100 Hz component if the amplitude in the following spectrum is provided as RMS values?</t>
+  </si>
+  <si>
+    <t>#power_converters</t>
+  </si>
+  <si>
+    <t>Power Converters</t>
+  </si>
+  <si>
+    <t>pc.2</t>
+  </si>
+  <si>
+    <t>What is the mean value of the signal in the following spectrum?</t>
+  </si>
+  <si>
+    <t>0 V. There is no component of 100 Hz (2nd harmonic)</t>
+  </si>
+  <si>
+    <t>5 V</t>
+  </si>
+  <si>
+    <t>pc.3</t>
+  </si>
+  <si>
+    <t>What is the peak value of the following signal?</t>
+  </si>
+  <si>
+    <t>150 V</t>
+  </si>
+  <si>
+    <t>&lt;img src="ed_block_diagram_01_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="ed_block_diagram_01_sol_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="spectrum_01_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="signal_01_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>pc.4</t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the switching times are:</t>
+  </si>
+  <si>
+    <t>[latex]$ t_{on-&gt;off} and t_{off-&gt;on}  $ [/latex] equal to 0 s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pc.5 </t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the equivalent resistance during the on state is:</t>
+  </si>
+  <si>
+    <t>[latex]$ R_{on}  $ [/latex] equal to 0 ohms.</t>
+  </si>
+  <si>
+    <t>pc.6</t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the equivalent resistance during the off state is:</t>
+  </si>
+  <si>
+    <t>pc.7</t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the power needed to change the state of the switch is:</t>
+  </si>
+  <si>
+    <t>0 W.</t>
+  </si>
+  <si>
+    <t>pc.8</t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the maximum voltage drop during the off state of the switch is:</t>
+  </si>
+  <si>
+    <t>[latex]$  \infty $[/latex]  V.</t>
+  </si>
+  <si>
+    <t>[latex]$ R_{off} -&gt; \infty $[/latex]  ohms.</t>
+  </si>
+  <si>
+    <t>pc.9</t>
+  </si>
+  <si>
+    <t>In an ideal power switch, the maximum current during the on state of the switch is:</t>
+  </si>
+  <si>
+    <t>[latex]$  \infty $[/latex]  A.</t>
+  </si>
+  <si>
+    <t>pc.10</t>
+  </si>
+  <si>
+    <t>What is the typical switching frequency and maximum power of an IGBT</t>
+  </si>
+  <si>
+    <t>[latex]$  f_s $[/latex] equal to 5 kHz and [latex]$ S_{max} $[/latex] equal to 10 kVA.</t>
+  </si>
+  <si>
+    <t>pc.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the typical switching frequency and maximum power of a Diode </t>
+  </si>
+  <si>
+    <t>[latex]$  f_s $[/latex] equal to 50 Hz and [latex]$ S_{max} $[/latex] equal to 10 MVA.</t>
+  </si>
+  <si>
+    <t>pc.12</t>
+  </si>
+  <si>
+    <t>What is the typical switching frequency and maximum power of a Mosfet</t>
+  </si>
+  <si>
+    <t>[latex]$  f_s $[/latex] equal to 100 kHz and [latex]$ S_{max} $[/latex] equal to 100 VA.</t>
+  </si>
+  <si>
+    <t>pc.13</t>
+  </si>
+  <si>
+    <t>What is the typical switching frequency and maximum power of a GTO</t>
+  </si>
+  <si>
+    <t>[latex]$  f_s $[/latex] equal to 100 Hz and [latex]$ S_{max} $[/latex] equal to 500 kVA.</t>
+  </si>
+  <si>
+    <t>pc.14</t>
+  </si>
+  <si>
+    <t>Which concept do you think is not related to a switched-mode power suppy: i) transformer; ii) high efficiency; iii) rectifier; iv) dc-dc converter; v) semiconductor operating in the linear region</t>
+  </si>
+  <si>
+    <t>pc.15</t>
+  </si>
+  <si>
+    <t>What semiconductor do your think is better for an inverter. A diode or a transistor?</t>
+  </si>
+  <si>
+    <t>v) semiconductor operating in the linear region.</t>
+  </si>
+  <si>
+    <t>A transistor, because you can control the moment when it is on or off.</t>
+  </si>
+  <si>
+    <t>m.1</t>
+  </si>
+  <si>
+    <t>The inertia of a rotating cilinder depends on:</t>
+  </si>
+  <si>
+    <t>mass and radius.</t>
+  </si>
+  <si>
+    <t>#mechanics</t>
+  </si>
+  <si>
+    <t>Mechanical requirements</t>
+  </si>
+  <si>
+    <t>sm.1</t>
+  </si>
+  <si>
+    <t>sm.2</t>
+  </si>
+  <si>
+    <t>What is the number of steps per revolution of a stepper motor with a stepper angle of 1.8 degrees per step?</t>
+  </si>
+  <si>
+    <t>200.</t>
+  </si>
+  <si>
+    <t>#stepper motor</t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>What is the pull-out torque?</t>
+  </si>
+  <si>
+    <t>Pull-out torque refers to the maximum torque that a stepper motor can generate while operating at a given speed before it loses synchronization with the input pulses, causing the motor to ”miss” steps or stall. When the motor’s load exceeds the pull-out torque, it can no longer maintain its designed step angle or speed, resulting in a loss of position accuracy. Pull-out torque decreases as the speed of the  motor increases due to the inherent characteristics of stepper motors.</t>
+  </si>
+  <si>
+    <t>sm.3</t>
+  </si>
+  <si>
+    <t>500 rpm</t>
+  </si>
+  <si>
+    <t>sm.4</t>
+  </si>
+  <si>
+    <t>Obtain the stepper angle of the following motor</t>
+  </si>
+  <si>
+    <t>&lt;img src="stepper_motor_02_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>What is the maximum no load starting speed in the following T vs speed torque?</t>
+  </si>
+  <si>
+    <t>&lt;img src="stepper_motor_01_mm.png"&gt;</t>
+  </si>
+  <si>
+    <t>10 degrees/step</t>
   </si>
 </sst>
 </file>
@@ -275,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,6 +519,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,27 +534,13 @@
   <dxfs count="60">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -323,6 +548,59 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -381,45 +659,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -676,15 +915,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{94DC8801-983D-49F6-B0DC-FCBD8A99C160}" name="eadmin222481012" displayName="eadmin222481012" ref="A1:J9" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2EF36E23-093B-45CE-B207-D7B8C13C7A5E}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{32026437-0B7A-4313-ADF1-D2EE57FE28B4}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{78005E75-F9DB-47E1-A18F-83788C9700B1}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6843DB7E-1219-450D-9C90-E382372B3F18}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{CB3496F4-AA64-4E44-8B7E-52B67BA29A72}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{51B9C059-A174-4F35-A3B8-D4CC73960CC3}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8E93FEFD-65A2-4C69-A537-109BE7B24728}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{0A857223-83D4-416D-A175-D7F259FB565A}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{C73A8F8F-87B3-4D7E-905D-B909484DEA34}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{D6F60A61-9CC2-46AB-AC7A-E3D32F190820}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{32026437-0B7A-4313-ADF1-D2EE57FE28B4}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{78005E75-F9DB-47E1-A18F-83788C9700B1}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6843DB7E-1219-450D-9C90-E382372B3F18}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{CB3496F4-AA64-4E44-8B7E-52B67BA29A72}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{51B9C059-A174-4F35-A3B8-D4CC73960CC3}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{8E93FEFD-65A2-4C69-A537-109BE7B24728}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{0A857223-83D4-416D-A175-D7F259FB565A}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{C73A8F8F-87B3-4D7E-905D-B909484DEA34}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{D6F60A61-9CC2-46AB-AC7A-E3D32F190820}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -781,25 +1020,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9131DEC1-BC7D-42C7-B2B6-1274C8482555}" name="eadmin2224" displayName="eadmin2224" ref="A1:J9" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9131DEC1-BC7D-42C7-B2B6-1274C8482555}" name="eadmin2224" displayName="eadmin2224" ref="A1:J16" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{40AFE8C3-BFBE-40AF-AEF8-CA82B0B5FDCC}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{E6B14D74-33DD-4739-96F8-CA3DBAADCA66}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{BABD5A33-01C7-462C-B535-554B660D96C9}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{EF254935-D5B9-4643-9A4F-21F889428E55}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="37" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{30B4E34F-1661-40B8-93E8-C0E885A9AE56}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{75FCC4B2-9ED3-4B29-97E9-FCCEF11DB81F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{35CD7FA6-E334-4472-B22D-E1F4E681B99E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{B0756186-91FF-4109-AE7C-D484C9762217}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{3DA56D1D-9D08-43A2-9C11-17DC615483B3}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{BD88878A-96B0-46D5-BAED-2A40990AB703}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{E6B14D74-33DD-4739-96F8-CA3DBAADCA66}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{BABD5A33-01C7-462C-B535-554B660D96C9}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EF254935-D5B9-4643-9A4F-21F889428E55}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="39" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{30B4E34F-1661-40B8-93E8-C0E885A9AE56}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{75FCC4B2-9ED3-4B29-97E9-FCCEF11DB81F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{35CD7FA6-E334-4472-B22D-E1F4E681B99E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{B0756186-91FF-4109-AE7C-D484C9762217}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{3DA56D1D-9D08-43A2-9C11-17DC615483B3}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{BD88878A-96B0-46D5-BAED-2A40990AB703}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7C859E2-95E3-4042-8B0C-4DDB370DE2C2}" name="Tabla537" displayName="Tabla537" ref="K1:Z9" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7C859E2-95E3-4042-8B0C-4DDB370DE2C2}" name="Tabla537" displayName="Tabla537" ref="K1:Z15" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{841FC890-EAFA-4B21-884E-11F076E98637}" name="Column11"/>
     <tableColumn id="2" xr3:uid="{2A59555E-F23D-419C-8A49-FC7403E70BAC}" name="Column12"/>
@@ -826,15 +1065,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{09911AA4-F774-4671-B766-AE97CB2642FB}" name="eadmin22248" displayName="eadmin22248" ref="A1:J9" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CFD18CDF-3847-49AD-8319-EEC6E94F3056}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{17E85D8C-A2CA-4421-ACB7-513170A2A397}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{5F34387C-0F35-4AEB-96DF-CEF85C9257EA}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{1EBF803E-B0FC-4447-9634-2A7D42A69A85}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="27" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{72970D14-2624-4B5B-A51E-E123CAA7D338}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{B6E5098F-3742-4C9D-B84D-FBF3F923068D}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{5E5CA604-AD49-48B6-BC85-93A458543E87}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{616BEA80-B72B-4CF4-BCA2-0A09A46BAE44}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{7DE79C54-D140-4789-8DE8-4B65D653983A}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{EE38240B-2FF8-4DC7-B40B-01945BE50076}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{17E85D8C-A2CA-4421-ACB7-513170A2A397}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{5F34387C-0F35-4AEB-96DF-CEF85C9257EA}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{1EBF803E-B0FC-4447-9634-2A7D42A69A85}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="29" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{72970D14-2624-4B5B-A51E-E123CAA7D338}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{B6E5098F-3742-4C9D-B84D-FBF3F923068D}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{5E5CA604-AD49-48B6-BC85-93A458543E87}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{616BEA80-B72B-4CF4-BCA2-0A09A46BAE44}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{7DE79C54-D140-4789-8DE8-4B65D653983A}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{EE38240B-2FF8-4DC7-B40B-01945BE50076}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -868,15 +1107,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{306FC542-01AC-4BA2-B1F1-9F4A67CDAFB6}" name="eadmin2224810" displayName="eadmin2224810" ref="A1:J9" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1AE80F45-7BD0-4A34-B701-BAB653688A1E}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{EDF5F641-2823-40B0-9436-00F4C0AC63E3}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{46069F46-A196-4136-9E25-41C63F91A1E0}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{6BDA5377-F35F-4E74-8B10-0FAADD36B079}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="17" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{33749FC4-59C1-4753-9EF5-F7A78B9BF2DA}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{EE6D55C2-5EB3-424C-A980-734004EE5606}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{B906A0D9-B94D-4586-996F-D2DE4880330E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{A416619C-C3BC-4875-B965-D345377D2EEE}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{9C166718-6BCA-4AD4-908E-206BB4C6466F}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{9207F911-613B-40D6-8F91-2C75BA55E2BD}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{EDF5F641-2823-40B0-9436-00F4C0AC63E3}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{46069F46-A196-4136-9E25-41C63F91A1E0}" uniqueName="11" name="Column22" queryTableFieldId="11" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{6BDA5377-F35F-4E74-8B10-0FAADD36B079}" uniqueName="3" name="Column3" queryTableFieldId="3" headerRowDxfId="19" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{33749FC4-59C1-4753-9EF5-F7A78B9BF2DA}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{EE6D55C2-5EB3-424C-A980-734004EE5606}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{B906A0D9-B94D-4586-996F-D2DE4880330E}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{A416619C-C3BC-4875-B965-D345377D2EEE}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{9C166718-6BCA-4AD4-908E-206BB4C6466F}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{9207F911-613B-40D6-8F91-2C75BA55E2BD}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1322,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DABDE3A-BB7B-4DC3-A6DB-DB47AB221C7D}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:T3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1334,7 +1573,7 @@
     <col min="2" max="2" width="62.265625" customWidth="1"/>
     <col min="3" max="3" width="80.53125" customWidth="1"/>
     <col min="4" max="4" width="80.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.796875" customWidth="1"/>
     <col min="7" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.19921875" bestFit="1" customWidth="1"/>
@@ -1409,6 +1648,29 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1422,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03862EA6-EC88-47BF-BD7F-204CCEEAD41D}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:W2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1441,7 +1703,7 @@
     <col min="11" max="16" width="10.796875" customWidth="1"/>
     <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="38.53125" customWidth="1"/>
-    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.59765625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="5" customWidth="1"/>
     <col min="24" max="26" width="5" bestFit="1" customWidth="1"/>
@@ -1509,6 +1771,26 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1521,16 +1803,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D560F21E-751A-4EBB-84D3-C71A8F603C7D}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="2" max="2" width="80.3984375" style="7" customWidth="1"/>
     <col min="3" max="3" width="80.53125" customWidth="1"/>
     <col min="4" max="4" width="80.53125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
@@ -1540,7 +1822,7 @@
     <col min="11" max="16" width="10.796875" customWidth="1"/>
     <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="38.53125" customWidth="1"/>
-    <col min="20" max="20" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="5" customWidth="1"/>
     <col min="24" max="26" width="5" bestFit="1" customWidth="1"/>
@@ -1550,7 +1832,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1607,6 +1889,367 @@
       <c r="T1" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="2" spans="1:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="Q10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="Q11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="Q12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="Q13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="Q14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="Q15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1818,16 +2461,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C6DE7D-6911-4F77-B121-8C60681D4BA5}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.265625" customWidth="1"/>
+    <col min="2" max="2" width="62.265625" style="7" customWidth="1"/>
     <col min="3" max="3" width="80.53125" customWidth="1"/>
     <col min="4" max="4" width="80.53125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.86328125" bestFit="1" customWidth="1"/>
@@ -1847,7 +2490,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1904,6 +2547,105 @@
       <c r="T1" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="2" spans="1:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>